<commit_message>
updated pleth breath types excel
</commit_message>
<xml_diff>
--- a/Pleth_Breath_Types/Pleth_breath_types.xlsx
+++ b/Pleth_Breath_Types/Pleth_breath_types.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.michaelson\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file.phhp.ufl.edu\data\home\edward.luca\Documents\Plethysmography\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,11 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">Sigh </t>
   </si>
   <si>
+    <t>Apnea</t>
+  </si>
+  <si>
     <t>Apnea Type I</t>
   </si>
   <si>
@@ -125,6 +128,9 @@
     <t>Notes:</t>
   </si>
   <si>
+    <t>Next 5 breaths after sigh</t>
+  </si>
+  <si>
     <t>&gt;300</t>
   </si>
   <si>
@@ -180,30 +186,6 @@
   </si>
   <si>
     <t>Non-respiratory sounds related to clearing the airways.</t>
-  </si>
-  <si>
-    <t>Apnea: 2 times greater or equal to average quiet breathing</t>
-  </si>
-  <si>
-    <t>Normal Apnea</t>
-  </si>
-  <si>
-    <t>10 breaths on either side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5-10 breaths </t>
-  </si>
-  <si>
-    <t>Immediately following sigh</t>
-  </si>
-  <si>
-    <t>30% of normal tidal volume. Lat at least 2 respiratory cycles.</t>
-  </si>
-  <si>
-    <t>Irregularity score below 15%, going for at least 100-200 breaths</t>
-  </si>
-  <si>
-    <t>Increase threshold of breath irregularity for acute injured rats</t>
   </si>
 </sst>
 </file>
@@ -538,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB73"/>
+  <dimension ref="A1:AA73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,90 +532,90 @@
     <col min="27" max="27" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -665,13 +647,13 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -686,7 +668,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -701,9 +683,9 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -731,15 +713,12 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -766,13 +745,10 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
-      <c r="AA5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -799,13 +775,10 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
-      <c r="AA6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -832,93 +805,77 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
-      <c r="AA7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AA30" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AA31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AA32" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AA33" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AA34" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AA35" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AA36" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AA37" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AA38" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="AA40" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update breath type excel
</commit_message>
<xml_diff>
--- a/Pleth_Breath_Types/Pleth_breath_types.xlsx
+++ b/Pleth_Breath_Types/Pleth_breath_types.xlsx
@@ -5,19 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edward.luca\Github\PlethMachineLearning\Pleth_Breath_Types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.michaelson\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Breath types" sheetId="1" r:id="rId1"/>
-    <sheet name="Sigh" sheetId="2" r:id="rId2"/>
-    <sheet name="Sniffing" sheetId="3" r:id="rId3"/>
-    <sheet name="Apnea Type I" sheetId="4" r:id="rId4"/>
-    <sheet name="Apnea Type II" sheetId="5" r:id="rId5"/>
-    <sheet name="Quiet Breathing" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t xml:space="preserve">Sigh </t>
   </si>
   <si>
-    <t>Apnea</t>
-  </si>
-  <si>
     <t>Apnea Type I</t>
   </si>
   <si>
@@ -133,9 +125,6 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Next 5 breaths after sigh</t>
-  </si>
-  <si>
     <t>&gt;300</t>
   </si>
   <si>
@@ -191,6 +180,30 @@
   </si>
   <si>
     <t>Non-respiratory sounds related to clearing the airways.</t>
+  </si>
+  <si>
+    <t>Apnea: 2 times greater or equal to average quiet breathing</t>
+  </si>
+  <si>
+    <t>Normal Apnea</t>
+  </si>
+  <si>
+    <t>10 breaths on either side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-10 breaths </t>
+  </si>
+  <si>
+    <t>Immediately following sigh</t>
+  </si>
+  <si>
+    <t>30% of normal tidal volume. Lat at least 2 respiratory cycles.</t>
+  </si>
+  <si>
+    <t>Irregularity score below 15%, going for at least 100-200 breaths</t>
+  </si>
+  <si>
+    <t>Increase threshold of breath irregularity for acute injured rats</t>
   </si>
 </sst>
 </file>
@@ -214,42 +227,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -264,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -274,26 +257,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA73"/>
+  <dimension ref="A1:AB73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,160 +550,160 @@
     <col min="27" max="27" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <v>550</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11">
-        <v>550</v>
-      </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11">
-        <v>5.5</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z2" s="11"/>
-    </row>
-    <row r="3" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -768,169 +731,194 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-    </row>
-    <row r="6" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-    </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AA30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AA31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AA32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AA34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AA35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AA36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AA37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AA38" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA40" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
@@ -940,64 +928,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>